<commit_message>
fix missing labels for dpv:Download, dpv:Export
thanks to Jenni Parry for reporting these
</commit_message>
<xml_diff>
--- a/code/vocab_csv/purpose_processing.xlsx
+++ b/code/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="1060">
   <si>
     <t>Term</t>
   </si>
@@ -18649,7 +18649,9 @@
       <c r="A59" s="45" t="s">
         <v>556</v>
       </c>
-      <c r="B59" s="61"/>
+      <c r="B59" s="45" t="s">
+        <v>556</v>
+      </c>
       <c r="C59" s="100" t="s">
         <v>557</v>
       </c>
@@ -18699,7 +18701,9 @@
       <c r="A60" s="45" t="s">
         <v>561</v>
       </c>
-      <c r="B60" s="61"/>
+      <c r="B60" s="45" t="s">
+        <v>561</v>
+      </c>
       <c r="C60" s="100" t="s">
         <v>562</v>
       </c>

</xml_diff>

<commit_message>
finalises HumanInvolvement concepts; closes #108
- does not include changes to documentation which will be implemented
  later for all changes introduced in v2
</commit_message>
<xml_diff>
--- a/code/vocab_csv/purpose_processing.xlsx
+++ b/code/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="1088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="1089">
   <si>
     <t>Term</t>
   </si>
@@ -2529,6 +2529,9 @@
   </si>
   <si>
     <t>Involvement where entity can reverse input of specified context</t>
+  </si>
+  <si>
+    <t>Reversion can be considered a form of correction in some instances. We welcome inputs to further explore and define this relation between correction and reversion concepts.</t>
   </si>
   <si>
     <t>EntityNonPermissiveInvolvement</t>
@@ -29953,7 +29956,9 @@
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
+      <c r="I40" s="45" t="s">
+        <v>737</v>
+      </c>
       <c r="J40" s="19"/>
       <c r="K40" s="46">
         <v>45423.0</v>
@@ -29982,13 +29987,13 @@
     </row>
     <row r="41">
       <c r="A41" s="69" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B41" s="61" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C41" s="100" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D41" s="116" t="s">
         <v>690</v>
@@ -30028,17 +30033,17 @@
     </row>
     <row r="42">
       <c r="A42" s="45" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B42" s="45" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C42" s="45" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -30072,17 +30077,17 @@
     </row>
     <row r="43">
       <c r="A43" s="45" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B43" s="45" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
@@ -30116,17 +30121,17 @@
     </row>
     <row r="44">
       <c r="A44" s="45" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B44" s="45" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -30160,17 +30165,17 @@
     </row>
     <row r="45">
       <c r="A45" s="45" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -30204,17 +30209,17 @@
     </row>
     <row r="46">
       <c r="A46" s="45" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B46" s="45" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
@@ -30250,17 +30255,17 @@
     </row>
     <row r="47">
       <c r="A47" s="45" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B47" s="45" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
@@ -30296,17 +30301,17 @@
     </row>
     <row r="48">
       <c r="A48" s="45" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B48" s="45" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C48" s="45" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
@@ -30340,17 +30345,17 @@
     </row>
     <row r="49">
       <c r="A49" s="45" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -30384,17 +30389,17 @@
     </row>
     <row r="50">
       <c r="A50" s="45" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B50" s="45" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C50" s="45" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
@@ -30430,17 +30435,17 @@
     </row>
     <row r="51">
       <c r="A51" s="45" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B51" s="45" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
@@ -30474,17 +30479,17 @@
     </row>
     <row r="52">
       <c r="A52" s="45" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B52" s="61" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
@@ -30518,17 +30523,17 @@
     </row>
     <row r="53">
       <c r="A53" s="45" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B53" s="61" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C53" s="45" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
@@ -30562,22 +30567,24 @@
     </row>
     <row r="54">
       <c r="A54" s="45" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B54" s="61" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C54" s="45" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D54" s="116"/>
       <c r="E54" s="45" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F54" s="19"/>
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
+      <c r="I54" s="45" t="s">
+        <v>737</v>
+      </c>
       <c r="J54" s="19"/>
       <c r="K54" s="46">
         <v>45423.0</v>
@@ -30609,13 +30616,13 @@
     </row>
     <row r="56">
       <c r="A56" s="45" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B56" s="45" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D56" s="116" t="s">
         <v>690</v>
@@ -30655,13 +30662,13 @@
     </row>
     <row r="57">
       <c r="A57" s="45" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B57" s="45" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C57" s="45" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D57" s="116" t="s">
         <v>690</v>
@@ -30701,13 +30708,13 @@
     </row>
     <row r="58">
       <c r="A58" s="45" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B58" s="45" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D58" s="116" t="s">
         <v>690</v>
@@ -30750,13 +30757,13 @@
     </row>
     <row r="60">
       <c r="A60" s="69" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B60" s="61" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C60" s="100" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="D60" s="116" t="s">
         <v>690</v>
@@ -30768,7 +30775,7 @@
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
       <c r="I60" s="107" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="J60" s="19"/>
       <c r="K60" s="46">
@@ -30802,23 +30809,23 @@
     </row>
     <row r="61">
       <c r="A61" s="45" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B61" s="45" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C61" s="100" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="D61" s="118"/>
       <c r="E61" s="116" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
       <c r="H61" s="19"/>
       <c r="I61" s="107" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="J61" s="105"/>
       <c r="K61" s="46">
@@ -30850,23 +30857,23 @@
     </row>
     <row r="62">
       <c r="A62" s="45" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B62" s="45" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C62" s="100" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="D62" s="118"/>
       <c r="E62" s="116" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
       <c r="H62" s="19"/>
       <c r="I62" s="107" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="J62" s="105"/>
       <c r="K62" s="46">
@@ -30898,23 +30905,23 @@
     </row>
     <row r="63">
       <c r="A63" s="45" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B63" s="45" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C63" s="100" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D63" s="118"/>
       <c r="E63" s="116" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F63" s="19"/>
       <c r="G63" s="19"/>
       <c r="H63" s="19"/>
       <c r="I63" s="107" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="J63" s="105"/>
       <c r="K63" s="46">
@@ -30946,23 +30953,23 @@
     </row>
     <row r="64">
       <c r="A64" s="45" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B64" s="45" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C64" s="100" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="D64" s="118"/>
       <c r="E64" s="116" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
       <c r="I64" s="107" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="J64" s="105"/>
       <c r="K64" s="46">
@@ -30994,23 +31001,23 @@
     </row>
     <row r="65">
       <c r="A65" s="45" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B65" s="45" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C65" s="100" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="D65" s="118"/>
       <c r="E65" s="116" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="19"/>
       <c r="H65" s="19"/>
       <c r="I65" s="107" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="J65" s="105"/>
       <c r="K65" s="46">
@@ -31044,23 +31051,23 @@
     </row>
     <row r="66">
       <c r="A66" s="45" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B66" s="45" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C66" s="100" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="D66" s="118"/>
       <c r="E66" s="116" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
       <c r="I66" s="107" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="J66" s="105"/>
       <c r="K66" s="46">
@@ -31094,23 +31101,23 @@
     </row>
     <row r="67">
       <c r="A67" s="45" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B67" s="45" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C67" s="100" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="D67" s="118"/>
       <c r="E67" s="116" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F67" s="19"/>
       <c r="G67" s="19"/>
       <c r="H67" s="19"/>
       <c r="I67" s="107" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="J67" s="105"/>
       <c r="K67" s="46">
@@ -31144,23 +31151,23 @@
     </row>
     <row r="68">
       <c r="A68" s="45" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B68" s="61" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C68" s="100" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="D68" s="45"/>
       <c r="E68" s="45" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F68" s="19"/>
       <c r="G68" s="19"/>
       <c r="H68" s="19"/>
       <c r="I68" s="107" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="J68" s="105"/>
       <c r="K68" s="46">
@@ -31204,7 +31211,7 @@
     </row>
     <row r="70">
       <c r="A70" s="69" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B70" s="61"/>
       <c r="C70" s="100"/>
@@ -31220,16 +31227,16 @@
     </row>
     <row r="71">
       <c r="A71" s="45" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B71" s="61" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C71" s="100" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="D71" s="45" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="E71" s="45" t="s">
         <v>18</v>
@@ -31238,7 +31245,7 @@
       <c r="G71" s="19"/>
       <c r="H71" s="19"/>
       <c r="I71" s="107" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="J71" s="105"/>
       <c r="K71" s="46">
@@ -31251,7 +31258,7 @@
         <v>23</v>
       </c>
       <c r="N71" s="45" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="O71" s="114"/>
       <c r="P71" s="19"/>
@@ -31272,13 +31279,13 @@
     </row>
     <row r="72">
       <c r="A72" s="114" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B72" s="115" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C72" s="119" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D72" s="45" t="s">
         <v>601</v>
@@ -31290,7 +31297,7 @@
       <c r="G72" s="19"/>
       <c r="H72" s="19"/>
       <c r="I72" s="120" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="J72" s="114"/>
       <c r="K72" s="46">
@@ -31324,16 +31331,16 @@
     </row>
     <row r="73">
       <c r="A73" s="45" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B73" s="61" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C73" s="100" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D73" s="45" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E73" s="45" t="s">
         <v>18</v>
@@ -31351,7 +31358,7 @@
         <v>23</v>
       </c>
       <c r="N73" s="45" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="O73" s="114"/>
       <c r="P73" s="19"/>
@@ -31372,16 +31379,16 @@
     </row>
     <row r="74">
       <c r="A74" s="45" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B74" s="61" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C74" s="100" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D74" s="45" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E74" s="45" t="s">
         <v>18</v>
@@ -31390,7 +31397,7 @@
       <c r="G74" s="19"/>
       <c r="H74" s="19"/>
       <c r="I74" s="107" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J74" s="114"/>
       <c r="K74" s="46">
@@ -31401,7 +31408,7 @@
         <v>23</v>
       </c>
       <c r="N74" s="45" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="O74" s="114"/>
       <c r="P74" s="19"/>
@@ -31422,16 +31429,16 @@
     </row>
     <row r="75">
       <c r="A75" s="45" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B75" s="61" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C75" s="100" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D75" s="45" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E75" s="45" t="s">
         <v>18</v>
@@ -31468,16 +31475,16 @@
     </row>
     <row r="76">
       <c r="A76" s="45" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B76" s="61" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C76" s="100" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="D76" s="45" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E76" s="45" t="s">
         <v>18</v>
@@ -31514,16 +31521,16 @@
     </row>
     <row r="77">
       <c r="A77" s="45" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B77" s="61" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C77" s="100" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="D77" s="45" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E77" s="45" t="s">
         <v>18</v>
@@ -31574,7 +31581,7 @@
     </row>
     <row r="79">
       <c r="A79" s="69" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B79" s="115"/>
       <c r="C79" s="100"/>
@@ -31590,13 +31597,13 @@
     </row>
     <row r="80">
       <c r="A80" s="114" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B80" s="115" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C80" s="100" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D80" s="25" t="s">
         <v>601</v>
@@ -31642,17 +31649,17 @@
     </row>
     <row r="81">
       <c r="A81" s="45" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B81" s="45" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C81" s="100" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D81" s="19"/>
       <c r="E81" s="45" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="F81" s="19"/>
       <c r="G81" s="19"/>
@@ -31692,17 +31699,17 @@
     </row>
     <row r="82">
       <c r="A82" s="45" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B82" s="45" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C82" s="100" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="D82" s="19"/>
       <c r="E82" s="45" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="F82" s="19"/>
       <c r="G82" s="19"/>
@@ -31742,23 +31749,23 @@
     </row>
     <row r="83">
       <c r="A83" s="45" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B83" s="61" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C83" s="100" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D83" s="45"/>
       <c r="E83" s="45" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="F83" s="19"/>
       <c r="G83" s="19"/>
       <c r="H83" s="19"/>
       <c r="I83" s="107" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="J83" s="105"/>
       <c r="K83" s="46">
@@ -31790,13 +31797,13 @@
     </row>
     <row r="84">
       <c r="A84" s="114" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B84" s="115" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C84" s="111" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D84" s="45" t="s">
         <v>601</v>
@@ -31838,13 +31845,13 @@
     </row>
     <row r="86">
       <c r="A86" s="9" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>17</v>
@@ -31856,7 +31863,7 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="122" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="10">
@@ -31870,7 +31877,7 @@
         <v>95</v>
       </c>
       <c r="O86" s="123" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="P86" s="8"/>
       <c r="Q86" s="8"/>
@@ -31890,13 +31897,13 @@
     </row>
     <row r="87">
       <c r="A87" s="69" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B87" s="61" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C87" s="100" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D87" s="25" t="s">
         <v>601</v>
@@ -31908,7 +31915,7 @@
       <c r="G87" s="19"/>
       <c r="H87" s="19"/>
       <c r="I87" s="107" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="J87" s="19"/>
       <c r="K87" s="46">
@@ -31938,17 +31945,17 @@
     </row>
     <row r="88">
       <c r="A88" s="45" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B88" s="61" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C88" s="100" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="45" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="F88" s="19"/>
       <c r="G88" s="19"/>
@@ -31982,23 +31989,23 @@
     </row>
     <row r="89">
       <c r="A89" s="114" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B89" s="115" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C89" s="100" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D89" s="19"/>
       <c r="E89" s="25" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="F89" s="19"/>
       <c r="G89" s="19"/>
       <c r="H89" s="19"/>
       <c r="I89" s="107" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="J89" s="106" t="s">
         <v>450</v>
@@ -32036,16 +32043,16 @@
     </row>
     <row r="91">
       <c r="A91" s="69" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B91" s="61" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C91" s="45" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="D91" s="45" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="E91" s="45" t="s">
         <v>596</v>
@@ -32063,7 +32070,7 @@
         <v>23</v>
       </c>
       <c r="N91" s="45" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="O91" s="124" t="s">
         <v>25</v>
@@ -32086,16 +32093,16 @@
     </row>
     <row r="92">
       <c r="A92" s="45" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B92" s="99" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="D92" s="45" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E92" s="45" t="s">
         <v>596</v>
@@ -32113,7 +32120,7 @@
         <v>23</v>
       </c>
       <c r="N92" s="45" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="O92" s="124" t="s">
         <v>25</v>
@@ -32136,16 +32143,16 @@
     </row>
     <row r="93">
       <c r="A93" s="45" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B93" s="99" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C93" s="69" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="D93" s="45" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E93" s="45" t="s">
         <v>596</v>
@@ -32163,7 +32170,7 @@
         <v>23</v>
       </c>
       <c r="N93" s="45" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="O93" s="124" t="s">
         <v>25</v>
@@ -32186,16 +32193,16 @@
     </row>
     <row r="94">
       <c r="A94" s="45" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B94" s="99" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="D94" s="45" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="E94" s="45" t="s">
         <v>596</v>
@@ -32213,7 +32220,7 @@
         <v>23</v>
       </c>
       <c r="N94" s="45" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="O94" s="124" t="s">
         <v>25</v>
@@ -32236,16 +32243,16 @@
     </row>
     <row r="95">
       <c r="A95" s="45" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B95" s="99" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="D95" s="45" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E95" s="45" t="s">
         <v>596</v>
@@ -32263,7 +32270,7 @@
         <v>23</v>
       </c>
       <c r="N95" s="45" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="O95" s="124" t="s">
         <v>25</v>
@@ -32286,13 +32293,13 @@
     </row>
     <row r="96">
       <c r="A96" s="114" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B96" s="115" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C96" s="119" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D96" s="19"/>
       <c r="E96" s="25" t="s">
@@ -32341,13 +32348,13 @@
     </row>
     <row r="98">
       <c r="A98" s="45" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B98" s="45" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C98" s="111" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="D98" s="45" t="s">
         <v>601</v>
@@ -32387,16 +32394,16 @@
     </row>
     <row r="99">
       <c r="A99" s="45" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B99" s="45" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C99" s="100" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="D99" s="45" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="E99" s="45" t="s">
         <v>596</v>
@@ -32435,16 +32442,16 @@
     </row>
     <row r="100">
       <c r="A100" s="45" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B100" s="45" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C100" s="100" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="D100" s="45" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="E100" s="45" t="s">
         <v>596</v>
@@ -37030,19 +37037,19 @@
     </row>
     <row r="2">
       <c r="A2" s="129" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B2" s="129" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C2" s="130" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="D2" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="129" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="F2" s="45" t="s">
         <v>430</v>
@@ -37059,7 +37066,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="129" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O2" s="133" t="s">
         <v>50</v>
@@ -37082,19 +37089,19 @@
     </row>
     <row r="3">
       <c r="A3" s="134" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="D3" s="134" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="134" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="F3" s="45" t="s">
         <v>430</v>
@@ -37103,7 +37110,7 @@
       <c r="H3" s="136"/>
       <c r="I3" s="136"/>
       <c r="J3" s="137" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="K3" s="132">
         <v>44786.0</v>
@@ -37113,7 +37120,7 @@
         <v>23</v>
       </c>
       <c r="N3" s="129" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="O3" s="139" t="s">
         <v>25</v>
@@ -37136,19 +37143,19 @@
     </row>
     <row r="4">
       <c r="A4" s="141" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B4" s="141" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C4" s="129" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="D4" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="129" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="F4" s="45" t="s">
         <v>430</v>
@@ -37167,7 +37174,7 @@
         <v>23</v>
       </c>
       <c r="N4" s="129" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O4" s="133" t="s">
         <v>101</v>
@@ -37190,13 +37197,13 @@
     </row>
     <row r="5">
       <c r="A5" s="45" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="D5" s="45" t="s">
         <v>17</v>
@@ -37242,19 +37249,19 @@
     </row>
     <row r="6">
       <c r="A6" s="141" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B6" s="141" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C6" s="129" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="D6" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F6" s="45" t="s">
         <v>430</v>
@@ -37262,7 +37269,7 @@
       <c r="G6" s="130"/>
       <c r="H6" s="130"/>
       <c r="I6" s="45" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="132">
@@ -37273,7 +37280,7 @@
         <v>23</v>
       </c>
       <c r="N6" s="129" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O6" s="133" t="s">
         <v>50</v>
@@ -37296,19 +37303,19 @@
     </row>
     <row r="7">
       <c r="A7" s="142" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B7" s="143" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="F7" s="40" t="s">
         <v>430</v>
@@ -37316,7 +37323,7 @@
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" s="144" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="J7" s="40"/>
       <c r="K7" s="145">
@@ -37329,7 +37336,7 @@
         <v>23</v>
       </c>
       <c r="N7" s="40" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="O7" s="146" t="s">
         <v>101</v>
@@ -37352,19 +37359,19 @@
     </row>
     <row r="8">
       <c r="A8" s="142" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B8" s="143" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="F8" s="40" t="s">
         <v>430</v>
@@ -37372,7 +37379,7 @@
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" s="144" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="J8" s="40"/>
       <c r="K8" s="145">
@@ -37385,10 +37392,10 @@
         <v>23</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="O8" s="146" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="P8" s="40"/>
       <c r="Q8" s="40"/>
@@ -37408,13 +37415,13 @@
     </row>
     <row r="9">
       <c r="A9" s="45" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C9" s="100" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="D9" s="45" t="s">
         <v>17</v>
@@ -37456,19 +37463,19 @@
     </row>
     <row r="10">
       <c r="A10" s="45" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C10" s="100" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D10" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="F10" s="45" t="s">
         <v>430</v>
@@ -37504,19 +37511,19 @@
     </row>
     <row r="11">
       <c r="A11" s="45" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C11" s="100" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="45" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="F11" s="45" t="s">
         <v>430</v>
@@ -37552,19 +37559,19 @@
     </row>
     <row r="12">
       <c r="A12" s="45" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="F12" s="45" t="s">
         <v>430</v>
@@ -37600,22 +37607,22 @@
     </row>
     <row r="13">
       <c r="A13" s="147" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B13" s="148" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C13" s="147" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="D13" s="147" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="147" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="F13" s="147" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
@@ -37650,19 +37657,19 @@
     </row>
     <row r="14">
       <c r="A14" s="45" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C14" s="100" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F14" s="45" t="s">
         <v>430</v>
@@ -37670,7 +37677,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
       <c r="I14" s="107" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
@@ -37698,19 +37705,19 @@
     </row>
     <row r="15">
       <c r="A15" s="45" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C15" s="100" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F15" s="45" t="s">
         <v>430</v>
@@ -37718,7 +37725,7 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="107" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
@@ -41702,13 +41709,13 @@
     </row>
     <row r="2">
       <c r="A2" s="45" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>601</v>
@@ -41720,7 +41727,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="107" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="46">
@@ -41731,7 +41738,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="45" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="O2" s="47" t="s">
         <v>101</v>
@@ -41764,16 +41771,16 @@
     </row>
     <row r="4">
       <c r="A4" s="69" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E4" s="45" t="s">
         <v>596</v>
@@ -41791,7 +41798,7 @@
         <v>23</v>
       </c>
       <c r="N4" s="45" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="O4" s="47" t="s">
         <v>101</v>
@@ -41812,17 +41819,17 @@
     </row>
     <row r="5">
       <c r="A5" s="45" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="45" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -41858,17 +41865,17 @@
     </row>
     <row r="6">
       <c r="A6" s="45" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="45" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -41904,17 +41911,17 @@
     </row>
     <row r="7">
       <c r="A7" s="45" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="45" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -41929,7 +41936,7 @@
         <v>23</v>
       </c>
       <c r="N7" s="45" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="O7" s="47" t="s">
         <v>101</v>
@@ -41950,17 +41957,17 @@
     </row>
     <row r="8">
       <c r="A8" s="45" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C8" s="100" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="45" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
@@ -41996,17 +42003,17 @@
     </row>
     <row r="9">
       <c r="A9" s="45" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C9" s="112" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="45" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -42042,17 +42049,17 @@
     </row>
     <row r="10">
       <c r="A10" s="45" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C10" s="100" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="45" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -42100,16 +42107,16 @@
     </row>
     <row r="12">
       <c r="A12" s="69" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E12" s="45" t="s">
         <v>596</v>
@@ -42127,7 +42134,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="45" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="O12" s="47" t="s">
         <v>101</v>
@@ -42148,17 +42155,17 @@
     </row>
     <row r="13">
       <c r="A13" s="45" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C13" s="113" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="45" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -42194,17 +42201,17 @@
     </row>
     <row r="14">
       <c r="A14" s="45" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C14" s="100" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="45" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
@@ -42240,17 +42247,17 @@
     </row>
     <row r="15">
       <c r="A15" s="45" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C15" s="100" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="45" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -42265,7 +42272,7 @@
         <v>23</v>
       </c>
       <c r="N15" s="45" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="O15" s="47" t="s">
         <v>101</v>
@@ -42286,17 +42293,17 @@
     </row>
     <row r="16">
       <c r="A16" s="45" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C16" s="100" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="45" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -42332,17 +42339,17 @@
     </row>
     <row r="17">
       <c r="A17" s="45" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C17" s="100" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="45" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
@@ -42378,17 +42385,17 @@
     </row>
     <row r="18">
       <c r="A18" s="45" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C18" s="100" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="45" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -42436,16 +42443,16 @@
     </row>
     <row r="20">
       <c r="A20" s="69" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C20" s="100" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E20" s="45" t="s">
         <v>596</v>
@@ -42463,7 +42470,7 @@
         <v>23</v>
       </c>
       <c r="N20" s="45" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="O20" s="47" t="s">
         <v>101</v>
@@ -42484,17 +42491,17 @@
     </row>
     <row r="21">
       <c r="A21" s="45" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C21" s="100" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
@@ -42530,17 +42537,17 @@
     </row>
     <row r="22">
       <c r="A22" s="45" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C22" s="100" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -42576,17 +42583,17 @@
     </row>
     <row r="23">
       <c r="A23" s="45" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C23" s="100" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -42622,17 +42629,17 @@
     </row>
     <row r="24">
       <c r="A24" s="45" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C24" s="100" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -42668,17 +42675,17 @@
     </row>
     <row r="25">
       <c r="A25" s="45" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C25" s="100" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -42714,23 +42721,23 @@
     </row>
     <row r="26">
       <c r="A26" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C26" s="100" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
       <c r="I26" s="107" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="J26" s="19"/>
       <c r="K26" s="46">
@@ -42762,23 +42769,23 @@
     </row>
     <row r="27">
       <c r="A27" s="45" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C27" s="100" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
       <c r="I27" s="107" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="J27" s="19"/>
       <c r="K27" s="46">
@@ -42821,16 +42828,16 @@
     </row>
     <row r="29">
       <c r="A29" s="69" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C29" s="100" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="D29" s="45" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E29" s="45" t="s">
         <v>596</v>
@@ -42839,7 +42846,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
       <c r="I29" s="151" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="J29" s="19"/>
       <c r="K29" s="46">
@@ -42869,23 +42876,23 @@
     </row>
     <row r="30">
       <c r="A30" s="153" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B30" s="154" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C30" s="155" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="156" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="F30" s="157"/>
       <c r="G30" s="157"/>
       <c r="H30" s="157"/>
       <c r="I30" s="151" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="J30" s="158" t="s">
         <v>450</v>
@@ -42923,17 +42930,17 @@
     </row>
     <row r="31">
       <c r="A31" s="45" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C31" s="100" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="114" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
@@ -42967,17 +42974,17 @@
     </row>
     <row r="32">
       <c r="A32" s="45" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B32" s="61" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C32" s="100" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="114" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -47795,19 +47802,19 @@
     </row>
     <row r="2">
       <c r="A2" s="45" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="F2" s="45" t="s">
         <v>430</v>
@@ -47845,22 +47852,22 @@
     </row>
     <row r="3">
       <c r="A3" s="45" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="D3" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -47877,7 +47884,7 @@
         <v>95</v>
       </c>
       <c r="O3" s="47" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
@@ -47895,22 +47902,22 @@
     </row>
     <row r="4">
       <c r="A4" s="45" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="D4" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="F4" s="45" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
@@ -47927,7 +47934,7 @@
         <v>95</v>
       </c>
       <c r="O4" s="47" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
@@ -47945,22 +47952,22 @@
     </row>
     <row r="5">
       <c r="A5" s="45" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="D5" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -47977,7 +47984,7 @@
         <v>95</v>
       </c>
       <c r="O5" s="47" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>

</xml_diff>

<commit_message>
fix typos in concepts, types, associations
- EU-GDPR added concept `AdequacyDecision` as an extension of A45-3, and
  the specific adequacy decisions are instances of this concept
- EU-GDPR added concept `DataProtectionAuthority` as an extension of DPV
  DataProtectionAuthority, and all DPAs are an instance of this concept
- EU-AIAct fixed typo in AIRegulatorySandbox parent "OrganisationMeasure"
  which should be "OrganisationalMeasure"
- Removed `dpv:Authority` from LEGAL-US, LEGAL-GB, and others as they
  are already defined as `dpv:DataProtectionAuthority`
- changed RDF generation so that laws and other legal concepts have a
  `skos:broader` triple added for their type e.g. `dpv:Law`
- RISK: added concept `RiskAnalysis` which is needed for the concept
  `RiskMatrix` and its instances
- DPV Processing Context: changed parent of hasStorageCondition from
  ProcessingCondition (which is class) to hasProcessingCondition
  (which is a property)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/purpose_processing.xlsx
+++ b/code/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1092">
   <si>
     <t>Term</t>
   </si>
@@ -3108,6 +3108,9 @@
   </si>
   <si>
     <t>Indicates information about storage condition</t>
+  </si>
+  <si>
+    <t>dpv:hasProcessingCondition</t>
   </si>
   <si>
     <r>
@@ -37160,13 +37163,13 @@
         <v>897</v>
       </c>
       <c r="F3" s="129" t="s">
-        <v>892</v>
+        <v>930</v>
       </c>
       <c r="G3" s="136"/>
       <c r="H3" s="136"/>
       <c r="I3" s="136"/>
       <c r="J3" s="137" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="K3" s="132">
         <v>44786.0</v>
@@ -37199,13 +37202,13 @@
     </row>
     <row r="4">
       <c r="A4" s="141" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B4" s="141" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C4" s="129" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="D4" s="129" t="s">
         <v>17</v>
@@ -37249,19 +37252,19 @@
     </row>
     <row r="5">
       <c r="A5" s="141" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B5" s="141" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C5" s="129" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="D5" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="129" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>430</v>
@@ -37303,13 +37306,13 @@
     </row>
     <row r="6">
       <c r="A6" s="46" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="D6" s="46" t="s">
         <v>17</v>
@@ -37355,13 +37358,13 @@
     </row>
     <row r="7">
       <c r="A7" s="141" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B7" s="141" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="D7" s="129" t="s">
         <v>17</v>
@@ -37375,7 +37378,7 @@
       <c r="G7" s="130"/>
       <c r="H7" s="130"/>
       <c r="I7" s="46" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="132">
@@ -37409,19 +37412,19 @@
     </row>
     <row r="8">
       <c r="A8" s="142" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B8" s="143" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="F8" s="40" t="s">
         <v>430</v>
@@ -37429,7 +37432,7 @@
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" s="144" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="J8" s="40"/>
       <c r="K8" s="145">
@@ -37442,7 +37445,7 @@
         <v>23</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="O8" s="146" t="s">
         <v>101</v>
@@ -37465,19 +37468,19 @@
     </row>
     <row r="9">
       <c r="A9" s="142" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B9" s="143" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="F9" s="40" t="s">
         <v>430</v>
@@ -37485,7 +37488,7 @@
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" s="144" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="J9" s="40"/>
       <c r="K9" s="145">
@@ -37498,7 +37501,7 @@
         <v>23</v>
       </c>
       <c r="N9" s="40" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="O9" s="146" t="s">
         <v>876</v>
@@ -37521,13 +37524,13 @@
     </row>
     <row r="10">
       <c r="A10" s="46" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C10" s="100" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>17</v>
@@ -37569,19 +37572,19 @@
     </row>
     <row r="11">
       <c r="A11" s="46" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C11" s="100" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="D11" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="F11" s="46" t="s">
         <v>430</v>
@@ -37617,19 +37620,19 @@
     </row>
     <row r="12">
       <c r="A12" s="46" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="D12" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="F12" s="46" t="s">
         <v>430</v>
@@ -37665,19 +37668,19 @@
     </row>
     <row r="13">
       <c r="A13" s="46" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C13" s="100" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="F13" s="46" t="s">
         <v>430</v>
@@ -37713,22 +37716,22 @@
     </row>
     <row r="14">
       <c r="A14" s="147" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B14" s="148" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C14" s="147" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="D14" s="147" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="147" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="F14" s="147" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
@@ -37763,19 +37766,19 @@
     </row>
     <row r="15">
       <c r="A15" s="46" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C15" s="100" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="D15" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>430</v>
@@ -37783,7 +37786,7 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="107" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
@@ -37811,19 +37814,19 @@
     </row>
     <row r="16">
       <c r="A16" s="46" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C16" s="100" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D16" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="F16" s="46" t="s">
         <v>430</v>
@@ -37831,7 +37834,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="107" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
@@ -41825,13 +41828,13 @@
     </row>
     <row r="2">
       <c r="A2" s="46" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>601</v>
@@ -41843,7 +41846,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="107" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="43">
@@ -41854,7 +41857,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="46" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="O2" s="47" t="s">
         <v>101</v>
@@ -41887,16 +41890,16 @@
     </row>
     <row r="4">
       <c r="A4" s="69" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>596</v>
@@ -41914,7 +41917,7 @@
         <v>23</v>
       </c>
       <c r="N4" s="46" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="O4" s="47" t="s">
         <v>101</v>
@@ -41935,17 +41938,17 @@
     </row>
     <row r="5">
       <c r="A5" s="46" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -41981,17 +41984,17 @@
     </row>
     <row r="6">
       <c r="A6" s="46" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -42027,17 +42030,17 @@
     </row>
     <row r="7">
       <c r="A7" s="46" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -42052,7 +42055,7 @@
         <v>23</v>
       </c>
       <c r="N7" s="46" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="O7" s="47" t="s">
         <v>101</v>
@@ -42073,17 +42076,17 @@
     </row>
     <row r="8">
       <c r="A8" s="46" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C8" s="100" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
@@ -42119,17 +42122,17 @@
     </row>
     <row r="9">
       <c r="A9" s="46" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C9" s="112" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -42165,17 +42168,17 @@
     </row>
     <row r="10">
       <c r="A10" s="46" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C10" s="100" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -42223,16 +42226,16 @@
     </row>
     <row r="12">
       <c r="A12" s="69" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E12" s="46" t="s">
         <v>596</v>
@@ -42250,7 +42253,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="O12" s="47" t="s">
         <v>101</v>
@@ -42271,17 +42274,17 @@
     </row>
     <row r="13">
       <c r="A13" s="46" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C13" s="113" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="46" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -42317,17 +42320,17 @@
     </row>
     <row r="14">
       <c r="A14" s="46" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C14" s="100" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="46" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
@@ -42363,17 +42366,17 @@
     </row>
     <row r="15">
       <c r="A15" s="46" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C15" s="100" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="46" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -42388,7 +42391,7 @@
         <v>23</v>
       </c>
       <c r="N15" s="46" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="O15" s="47" t="s">
         <v>101</v>
@@ -42409,17 +42412,17 @@
     </row>
     <row r="16">
       <c r="A16" s="46" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C16" s="100" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="46" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -42455,17 +42458,17 @@
     </row>
     <row r="17">
       <c r="A17" s="46" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C17" s="100" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="46" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
@@ -42501,17 +42504,17 @@
     </row>
     <row r="18">
       <c r="A18" s="46" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C18" s="100" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="46" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -42559,16 +42562,16 @@
     </row>
     <row r="20">
       <c r="A20" s="69" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C20" s="100" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E20" s="46" t="s">
         <v>596</v>
@@ -42586,7 +42589,7 @@
         <v>23</v>
       </c>
       <c r="N20" s="46" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="O20" s="47" t="s">
         <v>101</v>
@@ -42607,17 +42610,17 @@
     </row>
     <row r="21">
       <c r="A21" s="46" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C21" s="100" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
@@ -42653,17 +42656,17 @@
     </row>
     <row r="22">
       <c r="A22" s="46" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C22" s="100" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -42699,17 +42702,17 @@
     </row>
     <row r="23">
       <c r="A23" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C23" s="100" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -42745,17 +42748,17 @@
     </row>
     <row r="24">
       <c r="A24" s="46" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C24" s="100" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -42791,17 +42794,17 @@
     </row>
     <row r="25">
       <c r="A25" s="46" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C25" s="100" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -42837,23 +42840,23 @@
     </row>
     <row r="26">
       <c r="A26" s="46" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C26" s="100" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
       <c r="I26" s="107" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="J26" s="19"/>
       <c r="K26" s="43">
@@ -42885,23 +42888,23 @@
     </row>
     <row r="27">
       <c r="A27" s="46" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C27" s="100" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
       <c r="I27" s="107" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="J27" s="19"/>
       <c r="K27" s="43">
@@ -42944,16 +42947,16 @@
     </row>
     <row r="29">
       <c r="A29" s="69" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C29" s="100" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E29" s="46" t="s">
         <v>596</v>
@@ -42962,7 +42965,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
       <c r="I29" s="151" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="J29" s="19"/>
       <c r="K29" s="43">
@@ -42992,23 +42995,23 @@
     </row>
     <row r="30">
       <c r="A30" s="153" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B30" s="154" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C30" s="155" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="156" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="F30" s="157"/>
       <c r="G30" s="157"/>
       <c r="H30" s="157"/>
       <c r="I30" s="151" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="J30" s="158" t="s">
         <v>450</v>
@@ -43046,17 +43049,17 @@
     </row>
     <row r="31">
       <c r="A31" s="46" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C31" s="100" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="114" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
@@ -43090,17 +43093,17 @@
     </row>
     <row r="32">
       <c r="A32" s="46" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B32" s="61" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C32" s="100" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="114" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -47918,19 +47921,19 @@
     </row>
     <row r="2">
       <c r="A2" s="46" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>430</v>
@@ -47968,22 +47971,22 @@
     </row>
     <row r="3">
       <c r="A3" s="46" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -48000,7 +48003,7 @@
         <v>95</v>
       </c>
       <c r="O3" s="47" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
@@ -48018,22 +48021,22 @@
     </row>
     <row r="4">
       <c r="A4" s="46" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="D4" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
@@ -48050,7 +48053,7 @@
         <v>95</v>
       </c>
       <c r="O4" s="47" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
@@ -48068,22 +48071,22 @@
     </row>
     <row r="5">
       <c r="A5" s="46" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="D5" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -48100,7 +48103,7 @@
         <v>95</v>
       </c>
       <c r="O5" s="47" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>

</xml_diff>

<commit_message>
fix DPV Processing Context parent class/property
- DPV Processing Context EntityNonInvolvement did not have
  EntityInvolvement asserted as parent concept
- Same as above, hasActiveEntity, hasPassiveEntity, hasNonInvolvedEntity
  did not have hasEntity asserted as parent property
</commit_message>
<xml_diff>
--- a/code/vocab_csv/purpose_processing.xlsx
+++ b/code/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="1092">
   <si>
     <t>Term</t>
   </si>
@@ -3229,6 +3229,9 @@
     <t>dpv:EntityActiveInvolvement</t>
   </si>
   <si>
+    <t>dpv:hasEntity</t>
+  </si>
+  <si>
     <t>hasPassiveEntity</t>
   </si>
   <si>
@@ -3260,9 +3263,6 @@
   </si>
   <si>
     <t>Indicates the context is determined by the specified entity</t>
-  </si>
-  <si>
-    <t>dpv:hasEntity</t>
   </si>
   <si>
     <t>hasActiveDataSubject</t>
@@ -30776,7 +30776,9 @@
       <c r="D58" s="116" t="s">
         <v>689</v>
       </c>
-      <c r="E58" s="19"/>
+      <c r="E58" s="46" t="s">
+        <v>596</v>
+      </c>
       <c r="F58" s="19"/>
       <c r="G58" s="19"/>
       <c r="H58" s="19"/>
@@ -37586,8 +37588,8 @@
       <c r="E11" s="46" t="s">
         <v>964</v>
       </c>
-      <c r="F11" s="46" t="s">
-        <v>430</v>
+      <c r="F11" s="147" t="s">
+        <v>965</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -37620,22 +37622,22 @@
     </row>
     <row r="12">
       <c r="A12" s="46" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="D12" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>968</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>430</v>
+        <v>969</v>
+      </c>
+      <c r="F12" s="147" t="s">
+        <v>965</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -37668,22 +37670,22 @@
     </row>
     <row r="13">
       <c r="A13" s="46" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C13" s="100" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>972</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>430</v>
+        <v>973</v>
+      </c>
+      <c r="F13" s="147" t="s">
+        <v>965</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -37716,13 +37718,13 @@
     </row>
     <row r="14">
       <c r="A14" s="147" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B14" s="148" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C14" s="147" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="D14" s="147" t="s">
         <v>17</v>
@@ -37731,7 +37733,7 @@
         <v>955</v>
       </c>
       <c r="F14" s="147" t="s">
-        <v>976</v>
+        <v>965</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>

</xml_diff>

<commit_message>
fix usage notes in dpv rights
- fix usage notes in DPV rights concepts so they don't imply the reused
  property is restricted to rights concepts e.g. "Indicates X" -> "Also
  used for indicating X"
- added contributors to concepts in processing context, technical
  measures, tech provision
</commit_message>
<xml_diff>
--- a/code/vocab_csv/purpose_processing.xlsx
+++ b/code/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2386" uniqueCount="1094">
   <si>
     <t>Term</t>
   </si>
@@ -2402,6 +2402,9 @@
     <t>dpv:EntityPermissiveInvolvement</t>
   </si>
   <si>
+    <t>Harshvardhan J. Pandit, Delaram Golpayegani, Steve Hickman</t>
+  </si>
+  <si>
     <t>OptingOutFromProcess</t>
   </si>
   <si>
@@ -2667,6 +2670,9 @@
   </si>
   <si>
     <t>Involvement where entity is 'actively' involved</t>
+  </si>
+  <si>
+    <t>Delaram Golpayegani</t>
   </si>
   <si>
     <t>EntityPassiveInvolvement</t>
@@ -29392,7 +29398,9 @@
       <c r="M26" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N26" s="46"/>
+      <c r="N26" s="46" t="s">
+        <v>617</v>
+      </c>
       <c r="O26" s="46"/>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
@@ -29438,7 +29446,9 @@
       <c r="M27" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N27" s="46"/>
+      <c r="N27" s="46" t="s">
+        <v>617</v>
+      </c>
       <c r="O27" s="46"/>
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
@@ -29482,7 +29492,9 @@
       <c r="M28" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N28" s="19"/>
+      <c r="N28" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
@@ -29502,13 +29514,13 @@
     </row>
     <row r="29">
       <c r="A29" s="46" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="46" t="s">
@@ -29526,7 +29538,9 @@
       <c r="M29" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N29" s="19"/>
+      <c r="N29" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O29" s="19"/>
       <c r="P29" s="19"/>
       <c r="Q29" s="19"/>
@@ -29546,13 +29560,13 @@
     </row>
     <row r="30">
       <c r="A30" s="46" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="46" t="s">
@@ -29570,7 +29584,9 @@
       <c r="M30" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N30" s="19"/>
+      <c r="N30" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O30" s="19"/>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
@@ -29590,13 +29606,13 @@
     </row>
     <row r="31">
       <c r="A31" s="46" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="46" t="s">
@@ -29614,7 +29630,9 @@
       <c r="M31" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N31" s="19"/>
+      <c r="N31" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O31" s="19"/>
       <c r="P31" s="19"/>
       <c r="Q31" s="19"/>
@@ -29634,13 +29652,13 @@
     </row>
     <row r="32">
       <c r="A32" s="46" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="46" t="s">
@@ -29650,7 +29668,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
       <c r="I32" s="46" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="J32" s="19"/>
       <c r="K32" s="43">
@@ -29660,7 +29678,9 @@
       <c r="M32" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N32" s="19"/>
+      <c r="N32" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O32" s="19"/>
       <c r="P32" s="19"/>
       <c r="Q32" s="19"/>
@@ -29680,13 +29700,13 @@
     </row>
     <row r="33">
       <c r="A33" s="46" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="46" t="s">
@@ -29696,7 +29716,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
       <c r="I33" s="46" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="J33" s="19"/>
       <c r="K33" s="43">
@@ -29706,7 +29726,9 @@
       <c r="M33" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N33" s="19"/>
+      <c r="N33" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O33" s="19"/>
       <c r="P33" s="19"/>
       <c r="Q33" s="19"/>
@@ -29726,13 +29748,13 @@
     </row>
     <row r="34">
       <c r="A34" s="46" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="46" t="s">
@@ -29742,7 +29764,7 @@
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
       <c r="I34" s="46" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="J34" s="19"/>
       <c r="K34" s="43">
@@ -29752,7 +29774,9 @@
       <c r="M34" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N34" s="19"/>
+      <c r="N34" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
@@ -29772,13 +29796,13 @@
     </row>
     <row r="35">
       <c r="A35" s="46" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C35" s="46" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="46" t="s">
@@ -29788,7 +29812,7 @@
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
       <c r="I35" s="107" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="J35" s="19"/>
       <c r="K35" s="43">
@@ -29798,7 +29822,9 @@
       <c r="M35" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N35" s="19"/>
+      <c r="N35" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
@@ -29818,13 +29844,13 @@
     </row>
     <row r="36">
       <c r="A36" s="46" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C36" s="46" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="46" t="s">
@@ -29834,7 +29860,7 @@
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
       <c r="I36" s="46" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="J36" s="19"/>
       <c r="K36" s="43">
@@ -29844,7 +29870,9 @@
       <c r="M36" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N36" s="19"/>
+      <c r="N36" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
       <c r="Q36" s="19"/>
@@ -29864,13 +29892,13 @@
     </row>
     <row r="37">
       <c r="A37" s="46" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B37" s="61" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D37" s="116"/>
       <c r="E37" s="46" t="s">
@@ -29880,7 +29908,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
       <c r="I37" s="107" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="J37" s="19"/>
       <c r="K37" s="43">
@@ -29890,7 +29918,9 @@
       <c r="M37" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N37" s="46"/>
+      <c r="N37" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O37" s="46"/>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>
@@ -29910,13 +29940,13 @@
     </row>
     <row r="38">
       <c r="A38" s="46" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B38" s="61" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D38" s="116"/>
       <c r="E38" s="46" t="s">
@@ -29934,7 +29964,9 @@
       <c r="M38" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N38" s="46"/>
+      <c r="N38" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O38" s="46"/>
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
@@ -29954,13 +29986,13 @@
     </row>
     <row r="39">
       <c r="A39" s="46" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B39" s="61" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C39" s="46" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D39" s="116"/>
       <c r="E39" s="46" t="s">
@@ -29978,7 +30010,9 @@
       <c r="M39" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N39" s="46"/>
+      <c r="N39" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O39" s="46"/>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
@@ -29998,13 +30032,13 @@
     </row>
     <row r="40">
       <c r="A40" s="46" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B40" s="61" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D40" s="116"/>
       <c r="E40" s="46" t="s">
@@ -30014,7 +30048,7 @@
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
       <c r="I40" s="46" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="J40" s="19"/>
       <c r="K40" s="43">
@@ -30024,7 +30058,9 @@
       <c r="M40" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N40" s="46"/>
+      <c r="N40" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O40" s="46"/>
       <c r="P40" s="19"/>
       <c r="Q40" s="19"/>
@@ -30044,13 +30080,13 @@
     </row>
     <row r="41">
       <c r="A41" s="69" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B41" s="61" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C41" s="100" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D41" s="116" t="s">
         <v>689</v>
@@ -30070,7 +30106,9 @@
       <c r="M41" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N41" s="46"/>
+      <c r="N41" s="46" t="s">
+        <v>617</v>
+      </c>
       <c r="O41" s="46"/>
       <c r="P41" s="19"/>
       <c r="Q41" s="19"/>
@@ -30090,17 +30128,17 @@
     </row>
     <row r="42">
       <c r="A42" s="46" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -30114,7 +30152,9 @@
       <c r="M42" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N42" s="19"/>
+      <c r="N42" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O42" s="19"/>
       <c r="P42" s="19"/>
       <c r="Q42" s="19"/>
@@ -30134,17 +30174,17 @@
     </row>
     <row r="43">
       <c r="A43" s="46" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
@@ -30158,7 +30198,9 @@
       <c r="M43" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N43" s="19"/>
+      <c r="N43" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O43" s="19"/>
       <c r="P43" s="19"/>
       <c r="Q43" s="19"/>
@@ -30178,17 +30220,17 @@
     </row>
     <row r="44">
       <c r="A44" s="46" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B44" s="46" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -30202,7 +30244,9 @@
       <c r="M44" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N44" s="19"/>
+      <c r="N44" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O44" s="19"/>
       <c r="P44" s="19"/>
       <c r="Q44" s="19"/>
@@ -30222,17 +30266,17 @@
     </row>
     <row r="45">
       <c r="A45" s="46" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C45" s="46" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -30246,7 +30290,9 @@
       <c r="M45" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N45" s="19"/>
+      <c r="N45" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O45" s="19"/>
       <c r="P45" s="19"/>
       <c r="Q45" s="19"/>
@@ -30266,23 +30312,23 @@
     </row>
     <row r="46">
       <c r="A46" s="46" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C46" s="46" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
       <c r="H46" s="19"/>
       <c r="I46" s="46" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="J46" s="19"/>
       <c r="K46" s="43">
@@ -30292,7 +30338,9 @@
       <c r="M46" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N46" s="19"/>
+      <c r="N46" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
       <c r="Q46" s="19"/>
@@ -30312,23 +30360,23 @@
     </row>
     <row r="47">
       <c r="A47" s="46" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B47" s="46" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C47" s="46" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
       <c r="H47" s="19"/>
       <c r="I47" s="46" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="J47" s="19"/>
       <c r="K47" s="43">
@@ -30338,7 +30386,9 @@
       <c r="M47" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N47" s="19"/>
+      <c r="N47" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O47" s="19"/>
       <c r="P47" s="19"/>
       <c r="Q47" s="19"/>
@@ -30358,17 +30408,17 @@
     </row>
     <row r="48">
       <c r="A48" s="46" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C48" s="46" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
@@ -30382,7 +30432,9 @@
       <c r="M48" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N48" s="19"/>
+      <c r="N48" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
       <c r="Q48" s="19"/>
@@ -30402,17 +30454,17 @@
     </row>
     <row r="49">
       <c r="A49" s="46" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B49" s="46" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C49" s="46" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -30426,7 +30478,9 @@
       <c r="M49" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N49" s="19"/>
+      <c r="N49" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O49" s="19"/>
       <c r="P49" s="19"/>
       <c r="Q49" s="19"/>
@@ -30446,23 +30500,23 @@
     </row>
     <row r="50">
       <c r="A50" s="46" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B50" s="46" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C50" s="46" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
       <c r="H50" s="19"/>
       <c r="I50" s="46" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="J50" s="19"/>
       <c r="K50" s="43">
@@ -30472,7 +30526,9 @@
       <c r="M50" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N50" s="19"/>
+      <c r="N50" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O50" s="19"/>
       <c r="P50" s="19"/>
       <c r="Q50" s="19"/>
@@ -30492,17 +30548,17 @@
     </row>
     <row r="51">
       <c r="A51" s="46" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B51" s="46" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C51" s="46" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
@@ -30516,7 +30572,9 @@
       <c r="M51" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N51" s="19"/>
+      <c r="N51" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O51" s="19"/>
       <c r="P51" s="19"/>
       <c r="Q51" s="19"/>
@@ -30536,17 +30594,17 @@
     </row>
     <row r="52">
       <c r="A52" s="46" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B52" s="61" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
@@ -30560,7 +30618,9 @@
       <c r="M52" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N52" s="46"/>
+      <c r="N52" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O52" s="46"/>
       <c r="P52" s="19"/>
       <c r="Q52" s="19"/>
@@ -30580,17 +30640,17 @@
     </row>
     <row r="53">
       <c r="A53" s="46" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B53" s="61" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C53" s="46" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
@@ -30604,7 +30664,9 @@
       <c r="M53" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N53" s="46"/>
+      <c r="N53" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O53" s="46"/>
       <c r="P53" s="19"/>
       <c r="Q53" s="19"/>
@@ -30624,23 +30686,23 @@
     </row>
     <row r="54">
       <c r="A54" s="46" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B54" s="61" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C54" s="46" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D54" s="116"/>
       <c r="E54" s="46" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F54" s="19"/>
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
       <c r="I54" s="46" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="J54" s="19"/>
       <c r="K54" s="43">
@@ -30650,7 +30712,9 @@
       <c r="M54" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N54" s="46"/>
+      <c r="N54" s="46" t="s">
+        <v>694</v>
+      </c>
       <c r="O54" s="46"/>
       <c r="P54" s="19"/>
       <c r="Q54" s="19"/>
@@ -30673,13 +30737,13 @@
     </row>
     <row r="56">
       <c r="A56" s="46" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B56" s="46" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C56" s="46" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D56" s="116" t="s">
         <v>689</v>
@@ -30699,7 +30763,9 @@
       <c r="M56" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N56" s="19"/>
+      <c r="N56" s="46" t="s">
+        <v>784</v>
+      </c>
       <c r="O56" s="19"/>
       <c r="P56" s="19"/>
       <c r="Q56" s="19"/>
@@ -30719,13 +30785,13 @@
     </row>
     <row r="57">
       <c r="A57" s="46" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="B57" s="46" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="C57" s="46" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="D57" s="116" t="s">
         <v>689</v>
@@ -30745,7 +30811,9 @@
       <c r="M57" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N57" s="19"/>
+      <c r="N57" s="46" t="s">
+        <v>784</v>
+      </c>
       <c r="O57" s="19"/>
       <c r="P57" s="19"/>
       <c r="Q57" s="19"/>
@@ -30765,13 +30833,13 @@
     </row>
     <row r="58">
       <c r="A58" s="46" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B58" s="46" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="C58" s="46" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="D58" s="116" t="s">
         <v>689</v>
@@ -30791,7 +30859,9 @@
       <c r="M58" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="N58" s="19"/>
+      <c r="N58" s="46" t="s">
+        <v>784</v>
+      </c>
       <c r="O58" s="19"/>
       <c r="P58" s="19"/>
       <c r="Q58" s="19"/>
@@ -30816,13 +30886,13 @@
     </row>
     <row r="60">
       <c r="A60" s="69" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B60" s="61" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C60" s="100" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="D60" s="116" t="s">
         <v>689</v>
@@ -30834,7 +30904,7 @@
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
       <c r="I60" s="107" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="J60" s="19"/>
       <c r="K60" s="43">
@@ -30870,23 +30940,23 @@
     </row>
     <row r="61">
       <c r="A61" s="46" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C61" s="100" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="D61" s="118"/>
       <c r="E61" s="116" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
       <c r="H61" s="19"/>
       <c r="I61" s="107" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="J61" s="105"/>
       <c r="K61" s="43">
@@ -30918,23 +30988,23 @@
     </row>
     <row r="62">
       <c r="A62" s="46" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="C62" s="100" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="D62" s="118"/>
       <c r="E62" s="116" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
       <c r="H62" s="19"/>
       <c r="I62" s="107" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="J62" s="105"/>
       <c r="K62" s="43">
@@ -30966,23 +31036,23 @@
     </row>
     <row r="63">
       <c r="A63" s="46" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="C63" s="100" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="D63" s="118"/>
       <c r="E63" s="116" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F63" s="19"/>
       <c r="G63" s="19"/>
       <c r="H63" s="19"/>
       <c r="I63" s="107" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="J63" s="105"/>
       <c r="K63" s="43">
@@ -31014,23 +31084,23 @@
     </row>
     <row r="64">
       <c r="A64" s="46" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C64" s="100" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="D64" s="118"/>
       <c r="E64" s="116" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
       <c r="I64" s="107" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="J64" s="105"/>
       <c r="K64" s="43">
@@ -31062,23 +31132,23 @@
     </row>
     <row r="65">
       <c r="A65" s="46" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="C65" s="100" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="D65" s="118"/>
       <c r="E65" s="116" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="19"/>
       <c r="H65" s="19"/>
       <c r="I65" s="107" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="J65" s="105"/>
       <c r="K65" s="43">
@@ -31112,23 +31182,23 @@
     </row>
     <row r="66">
       <c r="A66" s="46" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C66" s="100" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="D66" s="118"/>
       <c r="E66" s="116" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
       <c r="I66" s="107" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="J66" s="105"/>
       <c r="K66" s="43">
@@ -31162,23 +31232,23 @@
     </row>
     <row r="67">
       <c r="A67" s="46" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="B67" s="46" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="C67" s="100" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="D67" s="118"/>
       <c r="E67" s="116" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F67" s="19"/>
       <c r="G67" s="19"/>
       <c r="H67" s="19"/>
       <c r="I67" s="107" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="J67" s="105"/>
       <c r="K67" s="43">
@@ -31212,23 +31282,23 @@
     </row>
     <row r="68">
       <c r="A68" s="46" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B68" s="61" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C68" s="100" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D68" s="46"/>
       <c r="E68" s="46" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F68" s="19"/>
       <c r="G68" s="19"/>
       <c r="H68" s="19"/>
       <c r="I68" s="107" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="J68" s="105"/>
       <c r="K68" s="43">
@@ -31272,7 +31342,7 @@
     </row>
     <row r="70">
       <c r="A70" s="69" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B70" s="61"/>
       <c r="C70" s="100"/>
@@ -31288,16 +31358,16 @@
     </row>
     <row r="71">
       <c r="A71" s="46" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="B71" s="61" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="C71" s="100" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="D71" s="46" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="E71" s="46" t="s">
         <v>18</v>
@@ -31306,7 +31376,7 @@
       <c r="G71" s="19"/>
       <c r="H71" s="19"/>
       <c r="I71" s="107" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="J71" s="105"/>
       <c r="K71" s="43">
@@ -31319,7 +31389,7 @@
         <v>23</v>
       </c>
       <c r="N71" s="46" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="O71" s="114"/>
       <c r="P71" s="19"/>
@@ -31340,13 +31410,13 @@
     </row>
     <row r="72">
       <c r="A72" s="114" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B72" s="115" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="C72" s="119" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="D72" s="46" t="s">
         <v>601</v>
@@ -31358,7 +31428,7 @@
       <c r="G72" s="19"/>
       <c r="H72" s="19"/>
       <c r="I72" s="120" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="J72" s="114"/>
       <c r="K72" s="43">
@@ -31392,16 +31462,16 @@
     </row>
     <row r="73">
       <c r="A73" s="46" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B73" s="61" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C73" s="100" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="D73" s="46" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="E73" s="46" t="s">
         <v>18</v>
@@ -31419,7 +31489,7 @@
         <v>23</v>
       </c>
       <c r="N73" s="46" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="O73" s="114"/>
       <c r="P73" s="19"/>
@@ -31440,16 +31510,16 @@
     </row>
     <row r="74">
       <c r="A74" s="46" t="s">
+        <v>843</v>
+      </c>
+      <c r="B74" s="61" t="s">
+        <v>844</v>
+      </c>
+      <c r="C74" s="100" t="s">
+        <v>845</v>
+      </c>
+      <c r="D74" s="46" t="s">
         <v>841</v>
-      </c>
-      <c r="B74" s="61" t="s">
-        <v>842</v>
-      </c>
-      <c r="C74" s="100" t="s">
-        <v>843</v>
-      </c>
-      <c r="D74" s="46" t="s">
-        <v>839</v>
       </c>
       <c r="E74" s="46" t="s">
         <v>18</v>
@@ -31458,7 +31528,7 @@
       <c r="G74" s="19"/>
       <c r="H74" s="19"/>
       <c r="I74" s="107" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="J74" s="114"/>
       <c r="K74" s="43">
@@ -31469,7 +31539,7 @@
         <v>23</v>
       </c>
       <c r="N74" s="46" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="O74" s="114"/>
       <c r="P74" s="19"/>
@@ -31490,16 +31560,16 @@
     </row>
     <row r="75">
       <c r="A75" s="46" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="B75" s="61" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="C75" s="100" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="D75" s="46" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="E75" s="46" t="s">
         <v>18</v>
@@ -31536,16 +31606,16 @@
     </row>
     <row r="76">
       <c r="A76" s="46" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B76" s="61" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="C76" s="100" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="D76" s="46" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="E76" s="46" t="s">
         <v>18</v>
@@ -31582,16 +31652,16 @@
     </row>
     <row r="77">
       <c r="A77" s="46" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="B77" s="61" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C77" s="100" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="D77" s="46" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="E77" s="46" t="s">
         <v>18</v>
@@ -31642,7 +31712,7 @@
     </row>
     <row r="79">
       <c r="A79" s="69" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B79" s="115"/>
       <c r="C79" s="100"/>
@@ -31658,13 +31728,13 @@
     </row>
     <row r="80">
       <c r="A80" s="114" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B80" s="115" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="C80" s="100" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="D80" s="25" t="s">
         <v>601</v>
@@ -31710,17 +31780,17 @@
     </row>
     <row r="81">
       <c r="A81" s="46" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="B81" s="46" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="C81" s="100" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="D81" s="19"/>
       <c r="E81" s="46" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="F81" s="19"/>
       <c r="G81" s="19"/>
@@ -31760,17 +31830,17 @@
     </row>
     <row r="82">
       <c r="A82" s="46" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="B82" s="46" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="C82" s="100" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="D82" s="19"/>
       <c r="E82" s="46" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="F82" s="19"/>
       <c r="G82" s="19"/>
@@ -31810,23 +31880,23 @@
     </row>
     <row r="83">
       <c r="A83" s="46" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="B83" s="61" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="C83" s="100" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="D83" s="46"/>
       <c r="E83" s="46" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="F83" s="19"/>
       <c r="G83" s="19"/>
       <c r="H83" s="19"/>
       <c r="I83" s="107" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="J83" s="105"/>
       <c r="K83" s="43">
@@ -31858,13 +31928,13 @@
     </row>
     <row r="84">
       <c r="A84" s="114" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="B84" s="115" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="C84" s="111" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="D84" s="46" t="s">
         <v>601</v>
@@ -31906,13 +31976,13 @@
     </row>
     <row r="86">
       <c r="A86" s="9" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>17</v>
@@ -31924,7 +31994,7 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="122" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="10">
@@ -31938,7 +32008,7 @@
         <v>95</v>
       </c>
       <c r="O86" s="123" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="P86" s="8"/>
       <c r="Q86" s="8"/>
@@ -31958,13 +32028,13 @@
     </row>
     <row r="87">
       <c r="A87" s="69" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="B87" s="61" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="C87" s="100" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D87" s="25" t="s">
         <v>601</v>
@@ -31976,7 +32046,7 @@
       <c r="G87" s="19"/>
       <c r="H87" s="19"/>
       <c r="I87" s="107" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="J87" s="19"/>
       <c r="K87" s="43">
@@ -32006,17 +32076,17 @@
     </row>
     <row r="88">
       <c r="A88" s="46" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B88" s="61" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C88" s="100" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="46" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="F88" s="19"/>
       <c r="G88" s="19"/>
@@ -32050,23 +32120,23 @@
     </row>
     <row r="89">
       <c r="A89" s="114" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="B89" s="115" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="C89" s="100" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="D89" s="19"/>
       <c r="E89" s="25" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="F89" s="19"/>
       <c r="G89" s="19"/>
       <c r="H89" s="19"/>
       <c r="I89" s="107" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="J89" s="106" t="s">
         <v>450</v>
@@ -32104,16 +32174,16 @@
     </row>
     <row r="91">
       <c r="A91" s="69" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="B91" s="61" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="C91" s="46" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="D91" s="46" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="E91" s="46" t="s">
         <v>596</v>
@@ -32131,7 +32201,7 @@
         <v>23</v>
       </c>
       <c r="N91" s="46" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="O91" s="124" t="s">
         <v>25</v>
@@ -32154,16 +32224,16 @@
     </row>
     <row r="92">
       <c r="A92" s="46" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="B92" s="99" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C92" s="46" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="D92" s="46" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="E92" s="46" t="s">
         <v>596</v>
@@ -32181,7 +32251,7 @@
         <v>23</v>
       </c>
       <c r="N92" s="46" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="O92" s="124" t="s">
         <v>25</v>
@@ -32204,16 +32274,16 @@
     </row>
     <row r="93">
       <c r="A93" s="46" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="B93" s="99" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="C93" s="46" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="D93" s="46" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="E93" s="46" t="s">
         <v>596</v>
@@ -32231,7 +32301,7 @@
         <v>23</v>
       </c>
       <c r="N93" s="46" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="O93" s="124" t="s">
         <v>25</v>
@@ -32254,16 +32324,16 @@
     </row>
     <row r="94">
       <c r="A94" s="46" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B94" s="99" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C94" s="46" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="D94" s="46" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="E94" s="46" t="s">
         <v>596</v>
@@ -32281,7 +32351,7 @@
         <v>23</v>
       </c>
       <c r="N94" s="46" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="O94" s="124" t="s">
         <v>25</v>
@@ -32304,16 +32374,16 @@
     </row>
     <row r="95">
       <c r="A95" s="46" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B95" s="99" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C95" s="46" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="D95" s="46" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="E95" s="46" t="s">
         <v>596</v>
@@ -32331,7 +32401,7 @@
         <v>23</v>
       </c>
       <c r="N95" s="46" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="O95" s="124" t="s">
         <v>25</v>
@@ -32354,13 +32424,13 @@
     </row>
     <row r="96">
       <c r="A96" s="114" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="B96" s="115" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C96" s="119" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="D96" s="19"/>
       <c r="E96" s="25" t="s">
@@ -32409,13 +32479,13 @@
     </row>
     <row r="98">
       <c r="A98" s="69" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="B98" s="46" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="C98" s="100" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="D98" s="46" t="s">
         <v>601</v>
@@ -32455,16 +32525,16 @@
     </row>
     <row r="99">
       <c r="A99" s="46" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B99" s="46" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C99" s="100" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="D99" s="46" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="E99" s="46" t="s">
         <v>596</v>
@@ -32503,16 +32573,16 @@
     </row>
     <row r="100">
       <c r="A100" s="46" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="B100" s="46" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C100" s="100" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="D100" s="46" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="E100" s="46" t="s">
         <v>596</v>
@@ -37098,19 +37168,19 @@
     </row>
     <row r="2">
       <c r="A2" s="129" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B2" s="129" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="C2" s="130" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="D2" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="129" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>430</v>
@@ -37127,7 +37197,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="129" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="O2" s="133" t="s">
         <v>50</v>
@@ -37150,28 +37220,28 @@
     </row>
     <row r="3">
       <c r="A3" s="134" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="D3" s="134" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="134" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="F3" s="129" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="G3" s="136"/>
       <c r="H3" s="136"/>
       <c r="I3" s="136"/>
       <c r="J3" s="137" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="K3" s="132">
         <v>44786.0</v>
@@ -37181,7 +37251,7 @@
         <v>23</v>
       </c>
       <c r="N3" s="129" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="O3" s="139" t="s">
         <v>25</v>
@@ -37204,19 +37274,19 @@
     </row>
     <row r="4">
       <c r="A4" s="141" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="B4" s="141" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="C4" s="129" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="D4" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="129" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="F4" s="46" t="s">
         <v>430</v>
@@ -37254,19 +37324,19 @@
     </row>
     <row r="5">
       <c r="A5" s="141" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B5" s="141" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="C5" s="129" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="D5" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="129" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>430</v>
@@ -37285,7 +37355,7 @@
         <v>23</v>
       </c>
       <c r="N5" s="129" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="O5" s="133" t="s">
         <v>101</v>
@@ -37308,13 +37378,13 @@
     </row>
     <row r="6">
       <c r="A6" s="46" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="D6" s="46" t="s">
         <v>17</v>
@@ -37360,19 +37430,19 @@
     </row>
     <row r="7">
       <c r="A7" s="141" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="B7" s="141" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="D7" s="129" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F7" s="46" t="s">
         <v>430</v>
@@ -37380,7 +37450,7 @@
       <c r="G7" s="130"/>
       <c r="H7" s="130"/>
       <c r="I7" s="46" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="132">
@@ -37391,7 +37461,7 @@
         <v>23</v>
       </c>
       <c r="N7" s="129" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="O7" s="133" t="s">
         <v>50</v>
@@ -37414,19 +37484,19 @@
     </row>
     <row r="8">
       <c r="A8" s="142" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="B8" s="143" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="F8" s="40" t="s">
         <v>430</v>
@@ -37434,7 +37504,7 @@
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" s="144" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="J8" s="40"/>
       <c r="K8" s="145">
@@ -37447,7 +37517,7 @@
         <v>23</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="O8" s="146" t="s">
         <v>101</v>
@@ -37470,19 +37540,19 @@
     </row>
     <row r="9">
       <c r="A9" s="142" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="B9" s="143" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="F9" s="40" t="s">
         <v>430</v>
@@ -37490,7 +37560,7 @@
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" s="144" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="J9" s="40"/>
       <c r="K9" s="145">
@@ -37503,10 +37573,10 @@
         <v>23</v>
       </c>
       <c r="N9" s="40" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="O9" s="146" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="P9" s="40"/>
       <c r="Q9" s="40"/>
@@ -37526,13 +37596,13 @@
     </row>
     <row r="10">
       <c r="A10" s="46" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="C10" s="100" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>17</v>
@@ -37574,22 +37644,22 @@
     </row>
     <row r="11">
       <c r="A11" s="46" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="C11" s="100" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="D11" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="F11" s="147" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -37622,22 +37692,22 @@
     </row>
     <row r="12">
       <c r="A12" s="46" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="D12" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="F12" s="147" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -37670,22 +37740,22 @@
     </row>
     <row r="13">
       <c r="A13" s="46" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="C13" s="100" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="F13" s="147" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -37718,22 +37788,22 @@
     </row>
     <row r="14">
       <c r="A14" s="147" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="B14" s="148" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="C14" s="147" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="D14" s="147" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="147" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="F14" s="147" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
@@ -37768,19 +37838,19 @@
     </row>
     <row r="15">
       <c r="A15" s="46" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C15" s="100" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="D15" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>430</v>
@@ -37788,7 +37858,7 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="107" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
@@ -37816,19 +37886,19 @@
     </row>
     <row r="16">
       <c r="A16" s="46" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="C16" s="100" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="D16" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="F16" s="46" t="s">
         <v>430</v>
@@ -37836,7 +37906,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="107" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
@@ -41830,13 +41900,13 @@
     </row>
     <row r="2">
       <c r="A2" s="46" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>601</v>
@@ -41848,7 +41918,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="107" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="43">
@@ -41859,7 +41929,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="46" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="O2" s="47" t="s">
         <v>101</v>
@@ -41892,16 +41962,16 @@
     </row>
     <row r="4">
       <c r="A4" s="69" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>596</v>
@@ -41919,7 +41989,7 @@
         <v>23</v>
       </c>
       <c r="N4" s="46" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="O4" s="47" t="s">
         <v>101</v>
@@ -41940,17 +42010,17 @@
     </row>
     <row r="5">
       <c r="A5" s="46" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="46" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -41986,17 +42056,17 @@
     </row>
     <row r="6">
       <c r="A6" s="46" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="46" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -42032,17 +42102,17 @@
     </row>
     <row r="7">
       <c r="A7" s="46" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="46" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -42057,7 +42127,7 @@
         <v>23</v>
       </c>
       <c r="N7" s="46" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="O7" s="47" t="s">
         <v>101</v>
@@ -42078,17 +42148,17 @@
     </row>
     <row r="8">
       <c r="A8" s="46" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="C8" s="100" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="46" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
@@ -42124,17 +42194,17 @@
     </row>
     <row r="9">
       <c r="A9" s="46" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="C9" s="112" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="46" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -42170,17 +42240,17 @@
     </row>
     <row r="10">
       <c r="A10" s="46" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="C10" s="100" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="46" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -42228,16 +42298,16 @@
     </row>
     <row r="12">
       <c r="A12" s="69" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E12" s="46" t="s">
         <v>596</v>
@@ -42255,7 +42325,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="46" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="O12" s="47" t="s">
         <v>101</v>
@@ -42276,17 +42346,17 @@
     </row>
     <row r="13">
       <c r="A13" s="46" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C13" s="113" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -42322,17 +42392,17 @@
     </row>
     <row r="14">
       <c r="A14" s="46" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="C14" s="100" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
@@ -42368,17 +42438,17 @@
     </row>
     <row r="15">
       <c r="A15" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="C15" s="100" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
@@ -42393,7 +42463,7 @@
         <v>23</v>
       </c>
       <c r="N15" s="46" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="O15" s="47" t="s">
         <v>101</v>
@@ -42414,17 +42484,17 @@
     </row>
     <row r="16">
       <c r="A16" s="46" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="C16" s="100" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -42460,17 +42530,17 @@
     </row>
     <row r="17">
       <c r="A17" s="46" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="C17" s="100" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
@@ -42506,17 +42576,17 @@
     </row>
     <row r="18">
       <c r="A18" s="46" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C18" s="100" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -42564,16 +42634,16 @@
     </row>
     <row r="20">
       <c r="A20" s="69" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="C20" s="100" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E20" s="46" t="s">
         <v>596</v>
@@ -42591,7 +42661,7 @@
         <v>23</v>
       </c>
       <c r="N20" s="46" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="O20" s="47" t="s">
         <v>101</v>
@@ -42612,17 +42682,17 @@
     </row>
     <row r="21">
       <c r="A21" s="46" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C21" s="100" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
@@ -42658,17 +42728,17 @@
     </row>
     <row r="22">
       <c r="A22" s="46" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C22" s="100" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -42704,17 +42774,17 @@
     </row>
     <row r="23">
       <c r="A23" s="46" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="C23" s="100" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
@@ -42750,17 +42820,17 @@
     </row>
     <row r="24">
       <c r="A24" s="46" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="C24" s="100" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -42796,17 +42866,17 @@
     </row>
     <row r="25">
       <c r="A25" s="46" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="C25" s="100" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -42842,23 +42912,23 @@
     </row>
     <row r="26">
       <c r="A26" s="46" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="C26" s="100" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
       <c r="I26" s="107" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="J26" s="19"/>
       <c r="K26" s="43">
@@ -42890,23 +42960,23 @@
     </row>
     <row r="27">
       <c r="A27" s="46" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C27" s="100" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
       <c r="I27" s="107" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="J27" s="19"/>
       <c r="K27" s="43">
@@ -42949,16 +43019,16 @@
     </row>
     <row r="29">
       <c r="A29" s="69" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="C29" s="100" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="E29" s="46" t="s">
         <v>596</v>
@@ -42967,7 +43037,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
       <c r="I29" s="151" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="J29" s="19"/>
       <c r="K29" s="43">
@@ -42997,23 +43067,23 @@
     </row>
     <row r="30">
       <c r="A30" s="153" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="B30" s="154" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C30" s="155" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="156" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="F30" s="157"/>
       <c r="G30" s="157"/>
       <c r="H30" s="157"/>
       <c r="I30" s="151" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="J30" s="158" t="s">
         <v>450</v>
@@ -43051,17 +43121,17 @@
     </row>
     <row r="31">
       <c r="A31" s="46" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="C31" s="100" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="114" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
@@ -43095,17 +43165,17 @@
     </row>
     <row r="32">
       <c r="A32" s="46" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="B32" s="61" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="C32" s="100" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="114" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -47923,19 +47993,19 @@
     </row>
     <row r="2">
       <c r="A2" s="46" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>430</v>
@@ -47973,22 +48043,22 @@
     </row>
     <row r="3">
       <c r="A3" s="46" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="D3" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -48005,7 +48075,7 @@
         <v>95</v>
       </c>
       <c r="O3" s="47" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
@@ -48023,22 +48093,22 @@
     </row>
     <row r="4">
       <c r="A4" s="46" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="D4" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
@@ -48055,7 +48125,7 @@
         <v>95</v>
       </c>
       <c r="O4" s="47" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
@@ -48073,22 +48143,22 @@
     </row>
     <row r="5">
       <c r="A5" s="46" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="D5" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -48105,7 +48175,7 @@
         <v>95</v>
       </c>
       <c r="O5" s="47" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>

</xml_diff>